<commit_message>
ajust in code calculate
</commit_message>
<xml_diff>
--- a/CalculateAMIB/GenerateCSV/StrutureData0.xlsx
+++ b/CalculateAMIB/GenerateCSV/StrutureData0.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell0\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MastersWork\MedicalDecisionSupport\CalculateAMIB\GenerateCSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C3713A-33E3-45E7-BF82-853B685BF526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF70880-43D7-4356-9C7F-BDDB102DED49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{97C584F9-C9E0-4BA7-80FE-11BDE73D0544}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{97C584F9-C9E0-4BA7-80FE-11BDE73D0544}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$3:$P$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$3:$O$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,15 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>Paciente</t>
   </si>
   <si>
     <t>idade</t>
-  </si>
-  <si>
-    <t>sexo</t>
   </si>
   <si>
     <t>SOFA</t>
@@ -354,22 +351,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -406,6 +388,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,13 +425,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>127470</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>128821</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>1051112</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>589</xdr:rowOff>
@@ -787,86 +784,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38BCAB35-9B63-4D48-9321-BCF0A5E95323}">
-  <dimension ref="A1:R31"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="5" customWidth="1"/>
     <col min="2" max="2" width="10.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.21875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="34.33203125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="53.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="25" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.5546875" style="5" customWidth="1"/>
-    <col min="15" max="15" width="11.109375" style="11" customWidth="1"/>
-    <col min="16" max="16" width="19.77734375" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="11"/>
+    <col min="3" max="3" width="13.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="34.33203125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="53.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="25" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5546875" style="5" customWidth="1"/>
+    <col min="14" max="14" width="11.109375" style="9" customWidth="1"/>
+    <col min="15" max="15" width="19.77734375" style="9" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="5" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9" t="s">
+    <row r="1" spans="1:17" s="5" customFormat="1" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="14"/>
-    </row>
-    <row r="2" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="24"/>
+      <c r="K1" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="27"/>
+    </row>
+    <row r="2" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -874,7 +868,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>4</v>
@@ -895,368 +889,344 @@
         <v>9</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="16">
+    </row>
+    <row r="4" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="11">
         <v>19</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="11">
         <v>0</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="11">
         <v>0</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="11">
+        <v>1</v>
+      </c>
+      <c r="F4" s="11">
+        <v>2</v>
+      </c>
+      <c r="G4" s="11">
+        <v>2</v>
+      </c>
+      <c r="H4" s="11">
+        <v>2</v>
+      </c>
+      <c r="I4" s="11">
+        <v>2</v>
+      </c>
+      <c r="J4" s="11">
+        <v>2</v>
+      </c>
+      <c r="K4" s="11">
+        <f>SUM(1+0+1)</f>
+        <v>2</v>
+      </c>
+      <c r="L4" s="11">
+        <v>2</v>
+      </c>
+      <c r="M4" s="11">
+        <f t="shared" ref="M4:M13" si="0">SUM(C4:H4)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="12">
+        <v>80</v>
+      </c>
+      <c r="C5" s="12">
         <v>0</v>
       </c>
-      <c r="F4" s="16">
+      <c r="D5" s="12">
+        <v>0</v>
+      </c>
+      <c r="E5" s="12">
+        <v>4</v>
+      </c>
+      <c r="F5" s="12">
+        <v>4</v>
+      </c>
+      <c r="G5" s="12">
+        <v>0</v>
+      </c>
+      <c r="H5" s="12">
         <v>1</v>
       </c>
-      <c r="G4" s="16">
-        <v>2</v>
-      </c>
-      <c r="H4" s="16">
-        <v>2</v>
-      </c>
-      <c r="I4" s="16">
-        <v>2</v>
-      </c>
-      <c r="J4" s="16">
-        <v>2</v>
-      </c>
-      <c r="K4" s="16">
-        <v>2</v>
-      </c>
-      <c r="L4" s="16">
-        <f>SUM(1+0+1)</f>
-        <v>2</v>
-      </c>
-      <c r="M4" s="16">
-        <v>2</v>
-      </c>
-      <c r="N4" s="16">
-        <f>SUM(D4:I4)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="17">
-        <v>80</v>
-      </c>
-      <c r="C5" s="17">
-        <v>0</v>
-      </c>
-      <c r="D5" s="17">
-        <v>0</v>
-      </c>
-      <c r="E5" s="17">
-        <v>0</v>
-      </c>
-      <c r="F5" s="17">
-        <v>4</v>
-      </c>
-      <c r="G5" s="17">
-        <v>4</v>
-      </c>
-      <c r="H5" s="17">
-        <v>0</v>
-      </c>
-      <c r="I5" s="17">
-        <v>1</v>
-      </c>
-      <c r="J5" s="17">
-        <v>4</v>
-      </c>
-      <c r="K5" s="17">
-        <v>2</v>
-      </c>
-      <c r="L5" s="17">
+      <c r="I5" s="12">
+        <v>4</v>
+      </c>
+      <c r="J5" s="12">
+        <v>2</v>
+      </c>
+      <c r="K5" s="12">
         <f>SUM(1+0+3)</f>
         <v>4</v>
       </c>
-      <c r="M5" s="17">
-        <v>2</v>
-      </c>
-      <c r="N5" s="17">
-        <f>SUM(D5:I5)</f>
+      <c r="L5" s="12">
+        <v>2</v>
+      </c>
+      <c r="M5" s="12">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="18">
+    <row r="6" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="13">
         <v>13</v>
       </c>
-      <c r="C6" s="18">
-        <v>1</v>
-      </c>
-      <c r="D6" s="18">
-        <v>4</v>
-      </c>
-      <c r="E6" s="18">
+      <c r="C6" s="13">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13">
         <v>3</v>
       </c>
-      <c r="F6" s="18">
-        <v>4</v>
-      </c>
-      <c r="G6" s="18">
-        <v>2</v>
-      </c>
-      <c r="H6" s="18">
-        <v>4</v>
-      </c>
-      <c r="I6" s="18">
+      <c r="E6" s="13">
+        <v>4</v>
+      </c>
+      <c r="F6" s="13">
+        <v>2</v>
+      </c>
+      <c r="G6" s="13">
+        <v>4</v>
+      </c>
+      <c r="H6" s="13">
         <v>3</v>
       </c>
-      <c r="J6" s="18">
-        <v>2</v>
-      </c>
-      <c r="K6" s="18">
-        <v>2</v>
-      </c>
-      <c r="L6" s="18">
+      <c r="I6" s="13">
+        <v>2</v>
+      </c>
+      <c r="J6" s="13">
+        <v>2</v>
+      </c>
+      <c r="K6" s="13">
         <f>SUM(4+0+1)</f>
         <v>5</v>
       </c>
-      <c r="M6" s="18">
-        <v>2</v>
-      </c>
-      <c r="N6" s="18">
-        <f>SUM(D6:I6)</f>
+      <c r="L6" s="13">
+        <v>2</v>
+      </c>
+      <c r="M6" s="13">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="8">
         <v>94</v>
       </c>
       <c r="C7" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="8">
+        <v>4</v>
+      </c>
+      <c r="E7" s="8">
         <v>0</v>
       </c>
-      <c r="E7" s="8">
-        <v>4</v>
-      </c>
       <c r="F7" s="8">
+        <v>3</v>
+      </c>
+      <c r="G7" s="8">
         <v>0</v>
       </c>
-      <c r="G7" s="8">
+      <c r="H7" s="8">
         <v>3</v>
       </c>
-      <c r="H7" s="8">
-        <v>0</v>
-      </c>
       <c r="I7" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J7" s="8">
-        <v>4</v>
-      </c>
-      <c r="K7" s="8">
-        <v>2</v>
-      </c>
-      <c r="L7" s="19">
+        <v>2</v>
+      </c>
+      <c r="K7" s="14">
         <f>SUM(2+0+4)</f>
         <v>6</v>
       </c>
-      <c r="M7" s="21">
-        <v>2</v>
-      </c>
-      <c r="N7" s="16">
-        <f>SUM(D7:I7)</f>
+      <c r="L7" s="16">
+        <v>2</v>
+      </c>
+      <c r="M7" s="11">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="8">
         <v>72</v>
       </c>
       <c r="C8" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="8">
+        <v>3</v>
+      </c>
+      <c r="E8" s="8">
+        <v>4</v>
+      </c>
+      <c r="F8" s="8">
+        <v>2</v>
+      </c>
+      <c r="G8" s="8">
         <v>0</v>
       </c>
-      <c r="E8" s="8">
-        <v>3</v>
-      </c>
-      <c r="F8" s="8">
-        <v>4</v>
-      </c>
-      <c r="G8" s="8">
-        <v>2</v>
-      </c>
       <c r="H8" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I8" s="8">
         <v>4</v>
       </c>
       <c r="J8" s="8">
-        <v>4</v>
-      </c>
-      <c r="K8" s="8">
-        <v>2</v>
-      </c>
-      <c r="L8" s="19">
+        <v>2</v>
+      </c>
+      <c r="K8" s="14">
         <f>SUM(3+0+3)</f>
         <v>6</v>
       </c>
-      <c r="M8" s="21">
-        <v>2</v>
-      </c>
-      <c r="N8" s="17">
-        <f>SUM(D8:I8)</f>
+      <c r="L8" s="16">
+        <v>2</v>
+      </c>
+      <c r="M8" s="12">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="8">
         <v>30</v>
       </c>
       <c r="C9" s="8">
+        <v>4</v>
+      </c>
+      <c r="D9" s="8">
+        <v>2</v>
+      </c>
+      <c r="E9" s="8">
         <v>1</v>
       </c>
-      <c r="D9" s="8">
-        <v>4</v>
-      </c>
-      <c r="E9" s="8">
-        <v>2</v>
-      </c>
       <c r="F9" s="8">
+        <v>0</v>
+      </c>
+      <c r="G9" s="8">
         <v>1</v>
-      </c>
-      <c r="G9" s="8">
-        <v>0</v>
       </c>
       <c r="H9" s="8">
         <v>1</v>
       </c>
       <c r="I9" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9" s="8">
-        <v>2</v>
-      </c>
-      <c r="K9" s="8">
-        <v>4</v>
-      </c>
-      <c r="L9" s="19">
+        <v>4</v>
+      </c>
+      <c r="K9" s="14">
         <f>SUM(2+3+1)</f>
         <v>6</v>
       </c>
-      <c r="M9" s="8">
-        <v>4</v>
-      </c>
-      <c r="N9" s="18">
-        <f>SUM(D9:I9)</f>
+      <c r="L9" s="8">
+        <v>4</v>
+      </c>
+      <c r="M9" s="13">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:18" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="24">
+    <row r="10" spans="1:17" s="20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="19">
         <v>46</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="19">
         <v>1</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="19">
+        <v>0</v>
+      </c>
+      <c r="E10" s="19">
+        <v>3</v>
+      </c>
+      <c r="F10" s="19">
         <v>1</v>
       </c>
-      <c r="E10" s="24">
-        <v>0</v>
-      </c>
-      <c r="F10" s="24">
+      <c r="G10" s="19">
         <v>3</v>
       </c>
-      <c r="G10" s="24">
-        <v>1</v>
-      </c>
-      <c r="H10" s="24">
-        <v>3</v>
-      </c>
-      <c r="I10" s="24">
-        <v>2</v>
-      </c>
-      <c r="J10" s="24">
-        <v>2</v>
-      </c>
-      <c r="K10" s="24">
-        <v>4</v>
-      </c>
-      <c r="L10" s="24">
+      <c r="H10" s="19">
+        <v>2</v>
+      </c>
+      <c r="I10" s="19">
+        <v>2</v>
+      </c>
+      <c r="J10" s="19">
+        <v>4</v>
+      </c>
+      <c r="K10" s="19">
         <f>SUM(2+3+2)</f>
         <v>7</v>
       </c>
-      <c r="M10" s="24">
-        <v>4</v>
-      </c>
-      <c r="N10" s="24">
-        <f>SUM(D10:I10)</f>
+      <c r="L10" s="19">
+        <v>4</v>
+      </c>
+      <c r="M10" s="19">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="24"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="8">
         <v>75</v>
       </c>
       <c r="C11" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D11" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E11" s="8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F11" s="8">
         <v>2</v>
@@ -1265,210 +1235,201 @@
         <v>2</v>
       </c>
       <c r="H11" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I11" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J11" s="8">
         <v>4</v>
       </c>
-      <c r="K11" s="8">
-        <v>4</v>
-      </c>
-      <c r="L11" s="20">
+      <c r="K11" s="15">
         <f>SUM(3+3+3)</f>
         <v>9</v>
       </c>
-      <c r="M11" s="22">
-        <v>4</v>
-      </c>
-      <c r="N11" s="26">
-        <f>SUM(D11:I11)</f>
+      <c r="L11" s="17">
+        <v>4</v>
+      </c>
+      <c r="M11" s="21">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="O11" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="N11" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="O11" s="22"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="8">
         <v>72</v>
       </c>
       <c r="C12" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D12" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E12" s="8">
+        <v>2</v>
+      </c>
+      <c r="F12" s="8">
+        <v>4</v>
+      </c>
+      <c r="G12" s="8">
         <v>1</v>
-      </c>
-      <c r="F12" s="8">
-        <v>2</v>
-      </c>
-      <c r="G12" s="8">
-        <v>4</v>
       </c>
       <c r="H12" s="8">
         <v>1</v>
       </c>
       <c r="I12" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12" s="8">
-        <v>2</v>
-      </c>
-      <c r="K12" s="8">
-        <v>4</v>
-      </c>
-      <c r="L12" s="20">
+        <v>4</v>
+      </c>
+      <c r="K12" s="15">
         <f>SUM(3+3+3)</f>
         <v>9</v>
       </c>
-      <c r="M12" s="22">
-        <v>4</v>
-      </c>
-      <c r="N12" s="26">
-        <f>SUM(D12:I12)</f>
+      <c r="L12" s="17">
+        <v>4</v>
+      </c>
+      <c r="M12" s="21">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="O12" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="N12" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="O12" s="22"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="8">
         <v>73</v>
       </c>
       <c r="C13" s="8">
+        <v>3</v>
+      </c>
+      <c r="D13" s="8">
         <v>0</v>
       </c>
-      <c r="D13" s="8">
+      <c r="E13" s="8">
+        <v>1</v>
+      </c>
+      <c r="F13" s="8">
+        <v>2</v>
+      </c>
+      <c r="G13" s="8">
+        <v>4</v>
+      </c>
+      <c r="H13" s="8">
         <v>3</v>
       </c>
-      <c r="E13" s="8">
-        <v>0</v>
-      </c>
-      <c r="F13" s="8">
-        <v>1</v>
-      </c>
-      <c r="G13" s="8">
-        <v>2</v>
-      </c>
-      <c r="H13" s="8">
-        <v>4</v>
-      </c>
       <c r="I13" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J13" s="8">
-        <v>2</v>
-      </c>
-      <c r="K13" s="8">
-        <v>4</v>
-      </c>
-      <c r="L13" s="20">
+        <v>4</v>
+      </c>
+      <c r="K13" s="15">
         <f>SUM(3+3+3)</f>
         <v>9</v>
       </c>
-      <c r="M13" s="22">
-        <v>4</v>
-      </c>
-      <c r="N13" s="26">
-        <f>SUM(D13:I13)</f>
+      <c r="L13" s="17">
+        <v>4</v>
+      </c>
+      <c r="M13" s="21">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="O13" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="23"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="N13" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="O13" s="22"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>41</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="J19"/>
       <c r="K19"/>
       <c r="L19"/>
-      <c r="M19"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="P22" s="11" t="s">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O22" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O24" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="P24" s="11" t="s">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O25" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="P25" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="P26" s="11" t="s">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O26" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O27" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O29" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O30" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="P27" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="P29" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="P30" s="11" t="s">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O31" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="P31" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A3:P3" xr:uid="{38BCAB35-9B63-4D48-9321-BCF0A5E95323}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:P13">
-      <sortCondition ref="L3"/>
+  <autoFilter ref="A3:O3" xr:uid="{38BCAB35-9B63-4D48-9321-BCF0A5E95323}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:O13">
+      <sortCondition ref="K3"/>
     </sortState>
   </autoFilter>
   <mergeCells count="6">
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>